<commit_message>
rebuilt tables and fixed discaRd issues
-rebuilt obs_prorate table
-rebuilt cams_catch_mock
-added region/halfofyear to mimic ACL accounting
-ran tests to compare squids against ACL accounting 2019
-identified issues with previous code using incorrect column for trip counts..
-KALL is relatively unaffected
-overall, illex is fairly close. seeing a drop in discard estimate but an increase in CV
-developed end to end run scheme making most things into functions

Co-Authored-By: Dan <danlinden@gmail.com>
</commit_message>
<xml_diff>
--- a/CAMS/SMB_FY2019_discRd_BG_example.xlsx
+++ b/CAMS/SMB_FY2019_discRd_BG_example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mack" sheetId="1" r:id="rId1"/>
@@ -323,12 +323,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -343,11 +349,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,25 +1408,25 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>1750</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>122</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>1.458214441496547E-2</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>21896431.973870799</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="2">
         <v>319296.93321545131</v>
       </c>
       <c r="H30">
@@ -1439,25 +1446,25 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>3019</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>375</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>0.12</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>4.0658350804005754E-3</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>25577560.136865132</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="2">
         <v>103994.1412755216</v>
       </c>
       <c r="H31">
@@ -1465,25 +1472,25 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>2530</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>211</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>0.08</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>1.6048277985198369E-3</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>29024889.379979141</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="2">
         <v>46579.949325953712</v>
       </c>
       <c r="H32">
@@ -1491,25 +1498,25 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>2346</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>432</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>0.18</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>9.3894767853846484E-5</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>33392176.301814649</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="2">
         <v>3135.3506419936002</v>
       </c>
       <c r="H33">
@@ -4455,9 +4462,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -5184,106 +5197,106 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>1750</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>122</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>2.1118282427345699E-3</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>21896431.973870799</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="2">
         <v>46241.503457536608</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="2">
         <v>0.41</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>3019</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>375</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>0.12</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>2.000886788871856E-2</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>25577560.136865132</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="2">
         <v>511778.02169428871</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="2">
         <v>0.34</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>2530</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>211</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>0.08</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>5.5523334435985628E-3</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>29024889.379979141</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="2">
         <v>161155.86400120691</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="2">
         <v>0.48</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>2346</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>432</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>0.18</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>2.5940985172919042E-3</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>33392176.301814649</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="2">
         <v>86622.595033687234</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="2">
         <v>0.31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
exploring mesh mismatches between obs and VTR
see the bottom of the MSB V2 module... it's significant
</commit_message>
<xml_diff>
--- a/CAMS/SMB_FY2019_discRd_BG_example.xlsx
+++ b/CAMS/SMB_FY2019_discRd_BG_example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="mack" sheetId="1" r:id="rId1"/>
@@ -306,7 +306,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +320,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -346,17 +357,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -661,13 +679,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:C30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A29" activePane="bottomLeft"/>
+      <selection activeCell="F1" sqref="F1:G1048576"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -687,10 +709,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -713,10 +735,10 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>2300</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>0</v>
       </c>
     </row>
@@ -736,10 +758,10 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>21469.262905162061</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -759,10 +781,10 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>753569.72512978013</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>0</v>
       </c>
       <c r="H4">
@@ -785,10 +807,10 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>700962.931795649</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>0</v>
       </c>
       <c r="H5">
@@ -811,10 +833,10 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>2452355.66145615</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>0</v>
       </c>
       <c r="H6">
@@ -837,10 +859,10 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>1761815.053452285</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>0</v>
       </c>
       <c r="H7">
@@ -863,10 +885,10 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>824600.54603952006</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>0</v>
       </c>
       <c r="H8">
@@ -889,10 +911,10 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>342935.35396048002</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>0</v>
       </c>
       <c r="H9">
@@ -915,10 +937,10 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>3597855.4026433248</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>0</v>
       </c>
       <c r="H10">
@@ -941,10 +963,10 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>371539.38865177229</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>0</v>
       </c>
       <c r="H11">
@@ -967,10 +989,10 @@
       <c r="E12">
         <v>2.6749104259039591E-6</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>2478138.821705427</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>6.6287993710171964</v>
       </c>
     </row>
@@ -990,10 +1012,10 @@
       <c r="E13">
         <v>1.158192941045663E-6</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>18322212.479166672</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>21.220657157709589</v>
       </c>
       <c r="H13">
@@ -1016,10 +1038,10 @@
       <c r="E14">
         <v>2.6749104259039591E-6</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>6774519.576923077</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <v>18.121233046802018</v>
       </c>
       <c r="H14">
@@ -1042,10 +1064,10 @@
       <c r="E15">
         <v>1.158192941045663E-6</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1065,10 +1087,10 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>38844786.131999999</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>0</v>
       </c>
       <c r="H16">
@@ -1091,10 +1113,10 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>15722</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1114,10 +1136,10 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>23373052.6192853</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>0</v>
       </c>
       <c r="H18">
@@ -1140,10 +1162,10 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>117464020.329</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>0</v>
       </c>
       <c r="H19">
@@ -1166,10 +1188,10 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>160428</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1189,10 +1211,10 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>22473219.009149559</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>0</v>
       </c>
       <c r="H21">
@@ -1215,10 +1237,10 @@
       <c r="E22">
         <v>2.2426049611471639E-4</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>36428091.839511126</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <v>8169.3819484412188</v>
       </c>
       <c r="H22">
@@ -1253,10 +1275,10 @@
       <c r="E23">
         <v>9.0540010726617291E-5</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>6906618.0694853142</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>625.32527409584918</v>
       </c>
       <c r="H23">
@@ -1279,10 +1301,10 @@
       <c r="E24">
         <v>7.1636957749213769E-6</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>31698095.08031968</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="3">
         <v>227.07550979994221</v>
       </c>
       <c r="H24">
@@ -1305,10 +1327,10 @@
       <c r="E25">
         <v>6.8115412806709478E-5</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>6413896.8770221323</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="3">
         <v>436.88523347802732</v>
       </c>
       <c r="H25">
@@ -1331,10 +1353,10 @@
       <c r="E26">
         <v>7.4032024555400911E-3</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>246476.5</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>1824.7154300329271</v>
       </c>
     </row>
@@ -1354,10 +1376,10 @@
       <c r="E27">
         <v>2.0781875455635969E-3</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>107667</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <v>223.75221846819571</v>
       </c>
     </row>
@@ -1377,10 +1399,10 @@
       <c r="E28">
         <v>1.6048277985198369E-3</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3">
         <v>68683.310872100425</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="3">
         <v>110.2248865819265</v>
       </c>
     </row>
@@ -1400,10 +1422,10 @@
       <c r="E29">
         <v>6.8115412806709478E-5</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3">
         <v>159857</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="3">
         <v>10.88872554504216</v>
       </c>
     </row>
@@ -1423,10 +1445,10 @@
       <c r="E30" s="2">
         <v>1.458214441496547E-2</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="5">
         <v>21896431.973870799</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="5">
         <v>319296.93321545131</v>
       </c>
       <c r="H30">
@@ -1461,10 +1483,10 @@
       <c r="E31" s="2">
         <v>4.0658350804005754E-3</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="5">
         <v>25577560.136865132</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="5">
         <v>103994.1412755216</v>
       </c>
       <c r="H31">
@@ -1487,10 +1509,10 @@
       <c r="E32" s="2">
         <v>1.6048277985198369E-3</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="5">
         <v>29024889.379979141</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="5">
         <v>46579.949325953712</v>
       </c>
       <c r="H32">
@@ -1513,10 +1535,10 @@
       <c r="E33" s="2">
         <v>9.3894767853846484E-5</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="5">
         <v>33392176.301814649</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="5">
         <v>3135.3506419936002</v>
       </c>
       <c r="H33">
@@ -1539,10 +1561,10 @@
       <c r="E34">
         <v>8.7544303628549482E-5</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="3">
         <v>2017068.655317503</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="3">
         <v>176.5828708007455</v>
       </c>
       <c r="H34">
@@ -1565,10 +1587,10 @@
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="3">
         <v>2115740.8440453699</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="3">
         <v>0</v>
       </c>
       <c r="H35">
@@ -1595,10 +1617,10 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="3">
         <v>564901.33666130423</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1618,10 +1640,10 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="3">
         <v>152326.6300376268</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1641,10 +1663,10 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="3">
         <v>1264097.995133939</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="3">
         <v>0</v>
       </c>
       <c r="H38">
@@ -1667,10 +1689,10 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="3">
         <v>167204.17654073989</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1690,10 +1712,10 @@
       <c r="E40">
         <v>3.3897660134232321E-4</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="3">
         <v>1519335.2860000001</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="3">
         <v>515.01911154774666</v>
       </c>
       <c r="H40">
@@ -1716,10 +1738,10 @@
       <c r="E41">
         <v>2.69092083310909E-5</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="3">
         <v>19051</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="3">
         <v>0.51264732791561285</v>
       </c>
     </row>
@@ -1739,10 +1761,10 @@
       <c r="E42">
         <v>2.69092083310909E-5</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="3">
         <v>564641.01</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="3">
         <v>15.19404257036758</v>
       </c>
       <c r="H42">
@@ -1765,10 +1787,10 @@
       <c r="E43">
         <v>0</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="3">
         <v>31608</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="3">
         <v>0</v>
       </c>
       <c r="H43">
@@ -1791,10 +1813,10 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="3">
         <v>202455.1253333333</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="3">
         <v>0</v>
       </c>
       <c r="H44">
@@ -1817,10 +1839,10 @@
       <c r="E45">
         <v>0</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="3">
         <v>301461.19276470592</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="3">
         <v>0</v>
       </c>
       <c r="H45">
@@ -1843,10 +1865,10 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="3">
         <v>248842.38373118901</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="3">
         <v>0</v>
       </c>
       <c r="H46">
@@ -1869,10 +1891,10 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="3">
         <v>792319</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="3">
         <v>0</v>
       </c>
       <c r="H47">
@@ -1895,10 +1917,10 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="3">
         <v>1172545</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="3">
         <v>0</v>
       </c>
       <c r="H48">
@@ -1921,10 +1943,10 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="3">
         <v>1892795</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1944,10 +1966,10 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="3">
         <v>20798650</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1967,10 +1989,10 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="3">
         <v>12748261</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="3">
         <v>0</v>
       </c>
       <c r="H51">
@@ -1993,10 +2015,10 @@
       <c r="E52">
         <v>0</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="3">
         <v>11330218</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2016,10 +2038,10 @@
       <c r="E53">
         <v>2.9647301005011441E-7</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="3">
         <v>184727530.00525001</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="3">
         <v>54.766726859779283</v>
       </c>
       <c r="H53">
@@ -2042,10 +2064,10 @@
       <c r="E54">
         <v>5.8254710335500052E-7</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="3">
         <v>79784042.78475</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="3">
         <v>46.477963018207539</v>
       </c>
       <c r="H54">
@@ -2068,10 +2090,10 @@
       <c r="E55">
         <v>0</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="3">
         <v>132614577.92729621</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="3">
         <v>0</v>
       </c>
       <c r="H55">
@@ -2094,10 +2116,10 @@
       <c r="E56">
         <v>0</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="3">
         <v>105493361.5907038</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="3">
         <v>0</v>
       </c>
       <c r="H56">
@@ -2120,10 +2142,10 @@
       <c r="E57">
         <v>2.4976470083808548E-5</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="3">
         <v>156123</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="3">
         <v>3.8994014388944409</v>
       </c>
     </row>
@@ -2143,10 +2165,10 @@
       <c r="E58">
         <v>2.4976470083808548E-5</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="3">
         <v>438704.72200000001</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="3">
         <v>10.957295364658551</v>
       </c>
       <c r="H58">
@@ -2169,10 +2191,10 @@
       <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="3">
         <v>640539.32499999995</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="3">
         <v>0</v>
       </c>
       <c r="H59">
@@ -2195,10 +2217,10 @@
       <c r="E60">
         <v>0</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="3">
         <v>79528</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2218,10 +2240,10 @@
       <c r="E61">
         <v>0</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="3">
         <v>619909.95116279065</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2241,10 +2263,10 @@
       <c r="E62">
         <v>0</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="3">
         <v>62199.4</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2264,10 +2286,10 @@
       <c r="E63">
         <v>0</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="3">
         <v>492005.245</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2287,10 +2309,10 @@
       <c r="E64">
         <v>2.707053483513985E-3</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="3">
         <v>913348.23580446152</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="3">
         <v>2472.48252339582</v>
       </c>
       <c r="H64">
@@ -2313,10 +2335,10 @@
       <c r="E65">
         <v>1.0600144396854239E-4</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="3">
         <v>5900901.001218589</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="3">
         <v>625.50402684458811</v>
       </c>
       <c r="H65">
@@ -2339,10 +2361,10 @@
       <c r="E66">
         <v>1.9758218340006759E-4</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="3">
         <v>4739632.0318539664</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="3">
         <v>936.46684536660541</v>
       </c>
       <c r="H66">
@@ -2365,10 +2387,10 @@
       <c r="E67">
         <v>6.9335785601398478E-6</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="3">
         <v>4326410.9030381572</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="3">
         <v>29.99750987966064</v>
       </c>
       <c r="H67">
@@ -2391,10 +2413,10 @@
       <c r="E68">
         <v>1.367946279792067E-3</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="3">
         <v>17226.322559848741</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="3">
         <v>23.56468386024325</v>
       </c>
     </row>
@@ -2414,10 +2436,10 @@
       <c r="E69">
         <v>5.4513088380210083E-5</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="3">
         <v>93717.001999999993</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="3">
         <v>5.1088032127543244</v>
       </c>
     </row>
@@ -2437,10 +2459,10 @@
       <c r="E70">
         <v>1.245375624931868E-4</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="3">
         <v>88026.33906281479</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="3">
         <v>10.96258570208175</v>
       </c>
     </row>
@@ -2460,10 +2482,10 @@
       <c r="E71">
         <v>3.4667892800699239E-6</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="3">
         <v>27117.873653330069</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="3">
         <v>9.40119536796553E-2</v>
       </c>
     </row>
@@ -2483,10 +2505,10 @@
       <c r="E72">
         <v>2.8839076070148979E-5</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="3">
         <v>8190024.8600657582</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="3">
         <v>236.19274995584769</v>
       </c>
       <c r="H72">
@@ -2509,10 +2531,10 @@
       <c r="E73">
         <v>3.0247327918777401E-6</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="3">
         <v>4353366.5807391303</v>
       </c>
-      <c r="G73">
+      <c r="G73" s="3">
         <v>13.16777065182632</v>
       </c>
       <c r="H73">
@@ -2535,10 +2557,10 @@
       <c r="E74">
         <v>5.1492941586306003E-5</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="3">
         <v>10837196.79415895</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="3">
         <v>558.03914148092917</v>
       </c>
       <c r="H74">
@@ -2561,10 +2583,10 @@
       <c r="E75">
         <v>0</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="3">
         <v>2139314.2969999998</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="3">
         <v>0</v>
       </c>
       <c r="H75">
@@ -2580,9 +2602,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2600,10 +2628,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -2626,10 +2654,10 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>2300</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2649,10 +2677,10 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>21469.262905162061</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2672,10 +2700,10 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>753569.72512978013</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>0</v>
       </c>
       <c r="H4">
@@ -2698,10 +2726,10 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>700962.931795649</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>0</v>
       </c>
       <c r="H5">
@@ -2724,10 +2752,10 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>2452355.66145615</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>0</v>
       </c>
       <c r="H6">
@@ -2750,10 +2778,10 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>1761815.053452285</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>0</v>
       </c>
       <c r="H7">
@@ -2776,10 +2804,10 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>824600.54603952006</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>0</v>
       </c>
       <c r="H8">
@@ -2802,10 +2830,10 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>342935.35396048002</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>0</v>
       </c>
       <c r="H9">
@@ -2828,10 +2856,10 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>3597855.4026433248</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>0</v>
       </c>
       <c r="H10">
@@ -2854,10 +2882,10 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>371539.38865177229</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>0</v>
       </c>
       <c r="H11">
@@ -2880,10 +2908,10 @@
       <c r="E12">
         <v>3.9336918027999386E-6</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>2478138.821705427</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>9.7482343691429367</v>
       </c>
     </row>
@@ -2903,10 +2931,10 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>18322212.479166672</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>0</v>
       </c>
       <c r="H13">
@@ -2929,10 +2957,10 @@
       <c r="E14">
         <v>3.9336918027999386E-6</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>6774519.576923077</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <v>26.648872127650019</v>
       </c>
       <c r="H14">
@@ -2955,10 +2983,10 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2978,10 +3006,10 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>38844786.131999999</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>0</v>
       </c>
       <c r="H16">
@@ -3004,10 +3032,10 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>15722</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>0</v>
       </c>
     </row>
@@ -3027,10 +3055,10 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>23373052.6192853</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>0</v>
       </c>
       <c r="H18">
@@ -3053,10 +3081,10 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>117464020.329</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>0</v>
       </c>
       <c r="H19">
@@ -3079,10 +3107,10 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>160428</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>0</v>
       </c>
     </row>
@@ -3102,10 +3130,10 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>22473219.009149559</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>0</v>
       </c>
       <c r="H21">
@@ -3128,10 +3156,10 @@
       <c r="E22">
         <v>1.3946194039676191E-4</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>36428091.839511126</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <v>5080.3323728896694</v>
       </c>
       <c r="H22">
@@ -3154,10 +3182,10 @@
       <c r="E23">
         <v>1.0415637952730001E-4</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>6906618.0694853142</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>719.36833289542005</v>
       </c>
       <c r="H23">
@@ -3180,10 +3208,10 @@
       <c r="E24">
         <v>1.5174450171877381E-3</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>31698095.08031968</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="3">
         <v>48100.116433974232</v>
       </c>
       <c r="H24">
@@ -3206,10 +3234,10 @@
       <c r="E25">
         <v>9.567656249728559E-5</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>6413896.8770221323</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="3">
         <v>613.65960540555295</v>
       </c>
       <c r="H25">
@@ -3232,10 +3260,10 @@
       <c r="E26">
         <v>5.1474061031380122E-3</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>246476.5</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>1268.7146403800959</v>
       </c>
     </row>
@@ -3255,10 +3283,10 @@
       <c r="E27">
         <v>3.2182618238282307E-2</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>107667</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <v>3465.0059578611422</v>
       </c>
     </row>
@@ -3278,10 +3306,10 @@
       <c r="E28">
         <v>5.3620337599451307E-3</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3">
         <v>68683.310872100425</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="3">
         <v>368.28223164100888</v>
       </c>
     </row>
@@ -3301,10 +3329,10 @@
       <c r="E29">
         <v>9.567656249728559E-5</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3">
         <v>159857</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="3">
         <v>15.294568251128579</v>
       </c>
     </row>
@@ -3324,10 +3352,10 @@
       <c r="E30">
         <v>1.015535026587926E-2</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="3">
         <v>21896431.973870799</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="3">
         <v>222365.93626765601</v>
       </c>
       <c r="H30">
@@ -3350,10 +3378,10 @@
       <c r="E31">
         <v>6.4261080097037321E-2</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="3">
         <v>25577560.136865132</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="3">
         <v>1643641.6406418791</v>
       </c>
       <c r="H31">
@@ -3376,10 +3404,10 @@
       <c r="E32">
         <v>5.3620337599451307E-3</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="3">
         <v>29024889.379979141</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="3">
         <v>155632.43673412109</v>
       </c>
       <c r="H32">
@@ -3402,10 +3430,10 @@
       <c r="E33">
         <v>5.4160942132072979E-3</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="3">
         <v>33392176.301814649</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="3">
         <v>180855.1728346562</v>
       </c>
       <c r="H33">
@@ -3428,10 +3456,10 @@
       <c r="E34">
         <v>3.8769620178357632E-4</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="3">
         <v>2017068.655317503</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="3">
         <v>782.00985640330168</v>
       </c>
       <c r="H34">
@@ -3454,10 +3482,10 @@
       <c r="E35">
         <v>1.39005339277192E-2</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="3">
         <v>2115740.8440453699</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="3">
         <v>29409.927384913921</v>
       </c>
       <c r="H35">
@@ -3480,10 +3508,10 @@
       <c r="E36">
         <v>6.4650379368426131E-2</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="3">
         <v>564901.33666130423</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="3">
         <v>36521.08572088433</v>
       </c>
     </row>
@@ -3503,10 +3531,10 @@
       <c r="E37">
         <v>6.4650379368426131E-2</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="3">
         <v>152326.6300376268</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="3">
         <v>9847.9744198464668</v>
       </c>
     </row>
@@ -3526,10 +3554,10 @@
       <c r="E38">
         <v>6.4650379368426131E-2</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="3">
         <v>1264097.995133939</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="3">
         <v>81724.414944276039</v>
       </c>
     </row>
@@ -3549,10 +3577,10 @@
       <c r="E39">
         <v>6.4650379368426131E-2</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="3">
         <v>167204.17654073989</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="3">
         <v>10809.813445344131</v>
       </c>
     </row>
@@ -3572,10 +3600,10 @@
       <c r="E40">
         <v>0.1799706854480175</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="3">
         <v>1519335.2860000001</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="3">
         <v>273435.81284677971</v>
       </c>
       <c r="H40">
@@ -3598,10 +3626,10 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="3">
         <v>19051</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="3">
         <v>0</v>
       </c>
     </row>
@@ -3621,10 +3649,10 @@
       <c r="E42">
         <v>0</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="3">
         <v>564641.01</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="3">
         <v>0</v>
       </c>
       <c r="H42">
@@ -3647,10 +3675,10 @@
       <c r="E43">
         <v>0</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="3">
         <v>31608</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="3">
         <v>0</v>
       </c>
       <c r="H43">
@@ -3673,10 +3701,10 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="3">
         <v>202455.1253333333</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="3">
         <v>0</v>
       </c>
       <c r="H44">
@@ -3699,10 +3727,10 @@
       <c r="E45">
         <v>0</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="3">
         <v>301461.19276470592</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="3">
         <v>0</v>
       </c>
       <c r="H45">
@@ -3725,10 +3753,10 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="3">
         <v>248842.38373118901</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="3">
         <v>0</v>
       </c>
       <c r="H46">
@@ -3751,10 +3779,10 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="3">
         <v>792319</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="3">
         <v>0</v>
       </c>
       <c r="H47">
@@ -3777,10 +3805,10 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="3">
         <v>1172545</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="3">
         <v>0</v>
       </c>
       <c r="H48">
@@ -3803,10 +3831,10 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="3">
         <v>1892795</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="3">
         <v>0</v>
       </c>
     </row>
@@ -3826,10 +3854,10 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="3">
         <v>20798650</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="3">
         <v>0</v>
       </c>
     </row>
@@ -3849,10 +3877,10 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="3">
         <v>12748261</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="3">
         <v>0</v>
       </c>
       <c r="H51">
@@ -3875,10 +3903,10 @@
       <c r="E52">
         <v>0</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="3">
         <v>11330218</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="3">
         <v>0</v>
       </c>
     </row>
@@ -3898,10 +3926,10 @@
       <c r="E53">
         <v>2.4508435497476118E-6</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="3">
         <v>184727530.00525001</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="3">
         <v>452.73827537417549</v>
       </c>
       <c r="H53">
@@ -3924,10 +3952,10 @@
       <c r="E54">
         <v>7.4436574317583404E-7</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="3">
         <v>79784042.78475</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="3">
         <v>59.388508301042982</v>
       </c>
       <c r="H54">
@@ -3950,10 +3978,10 @@
       <c r="E55">
         <v>7.3578403968243425E-5</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="3">
         <v>132614577.92729621</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="3">
         <v>9757.5689868126956</v>
       </c>
       <c r="H55">
@@ -3976,10 +4004,10 @@
       <c r="E56">
         <v>3.4040599923819719E-6</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="3">
         <v>105493361.5907038</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="3">
         <v>359.10573165279988</v>
       </c>
       <c r="H56">
@@ -4002,10 +4030,10 @@
       <c r="E57">
         <v>0</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="3">
         <v>156123</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4025,10 +4053,10 @@
       <c r="E58">
         <v>0</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="3">
         <v>438704.72200000001</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="3">
         <v>0</v>
       </c>
       <c r="H58">
@@ -4051,10 +4079,10 @@
       <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="3">
         <v>640539.32499999995</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="3">
         <v>0</v>
       </c>
       <c r="H59">
@@ -4077,10 +4105,10 @@
       <c r="E60">
         <v>0</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="3">
         <v>79528</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4100,10 +4128,10 @@
       <c r="E61">
         <v>0</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="3">
         <v>619909.95116279065</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4123,10 +4151,10 @@
       <c r="E62">
         <v>0</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="3">
         <v>62199.4</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4146,10 +4174,10 @@
       <c r="E63">
         <v>0</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="3">
         <v>492005.245</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4169,10 +4197,10 @@
       <c r="E64">
         <v>0</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="3">
         <v>913348.23580446152</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="3">
         <v>0</v>
       </c>
       <c r="H64">
@@ -4195,10 +4223,10 @@
       <c r="E65">
         <v>0</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="3">
         <v>5900901.001218589</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="3">
         <v>0</v>
       </c>
       <c r="H65">
@@ -4221,10 +4249,10 @@
       <c r="E66">
         <v>7.7301323708946637E-7</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="3">
         <v>4739632.0318539664</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="3">
         <v>3.6637982995563592</v>
       </c>
       <c r="H66">
@@ -4247,10 +4275,10 @@
       <c r="E67">
         <v>0</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="3">
         <v>4326410.9030381572</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="3">
         <v>0</v>
       </c>
       <c r="H67">
@@ -4273,10 +4301,10 @@
       <c r="E68">
         <v>3.2043417855721092E-7</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="3">
         <v>17226.322559848741</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="3">
         <v>5.519902519026682E-3</v>
       </c>
     </row>
@@ -4296,10 +4324,10 @@
       <c r="E69">
         <v>0</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="3">
         <v>93717.001999999993</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4319,10 +4347,10 @@
       <c r="E70">
         <v>3.8650661854473319E-7</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="3">
         <v>88026.33906281479</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="3">
         <v>3.4022762654040702E-2</v>
       </c>
     </row>
@@ -4342,10 +4370,10 @@
       <c r="E71">
         <v>0</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="3">
         <v>27117.873653330069</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4365,10 +4393,10 @@
       <c r="E72">
         <v>6.4086835711442173E-7</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="3">
         <v>8190024.8600657582</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="3">
         <v>5.2487277767966143</v>
       </c>
       <c r="H72">
@@ -4391,10 +4419,10 @@
       <c r="E73">
         <v>0</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="3">
         <v>4353366.5807391303</v>
       </c>
-      <c r="G73">
+      <c r="G73" s="3">
         <v>0</v>
       </c>
       <c r="H73">
@@ -4417,10 +4445,10 @@
       <c r="E74">
         <v>0</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="3">
         <v>10837196.79415895</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="3">
         <v>0</v>
       </c>
       <c r="H74">
@@ -4443,10 +4471,10 @@
       <c r="E75">
         <v>0</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="3">
         <v>2139314.2969999998</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="3">
         <v>0</v>
       </c>
       <c r="H75">
@@ -4462,14 +4490,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="765" topLeftCell="A2"/>
+      <selection activeCell="F1" sqref="F1:G1048576"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4488,10 +4519,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -4514,10 +4545,10 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>2300</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4537,10 +4568,10 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>21469.262905162061</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4560,10 +4591,10 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>753569.72512978013</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>0</v>
       </c>
       <c r="H4">
@@ -4586,10 +4617,10 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>700962.931795649</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>0</v>
       </c>
       <c r="H5">
@@ -4612,10 +4643,10 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>2452355.66145615</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>0</v>
       </c>
       <c r="H6">
@@ -4638,10 +4669,10 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>1761815.053452285</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>0</v>
       </c>
       <c r="H7">
@@ -4664,10 +4695,10 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>824600.54603952006</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>0</v>
       </c>
       <c r="H8">
@@ -4690,10 +4721,10 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>342935.35396048002</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>0</v>
       </c>
       <c r="H9">
@@ -4716,10 +4747,10 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>3597855.4026433248</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>0</v>
       </c>
       <c r="H10">
@@ -4742,10 +4773,10 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>371539.38865177229</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>0</v>
       </c>
       <c r="H11">
@@ -4768,10 +4799,10 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>2478138.821705427</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4791,10 +4822,10 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>18322212.479166672</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>0</v>
       </c>
       <c r="H13">
@@ -4817,10 +4848,10 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>6774519.576923077</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <v>0</v>
       </c>
       <c r="H14">
@@ -4843,10 +4874,10 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4866,10 +4897,10 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>38844786.131999999</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>0</v>
       </c>
       <c r="H16">
@@ -4892,10 +4923,10 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>15722</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4915,10 +4946,10 @@
       <c r="E18">
         <v>1.836368364239625E-7</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>23373052.6192853</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>4.2921534405763637</v>
       </c>
       <c r="H18">
@@ -4941,10 +4972,10 @@
       <c r="E19">
         <v>1.140459242050621E-7</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>117464020.329</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>13.396292759263011</v>
       </c>
       <c r="H19">
@@ -4967,10 +4998,10 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>160428</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4990,10 +5021,10 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>22473219.009149559</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>0</v>
       </c>
       <c r="H21">
@@ -5016,10 +5047,10 @@
       <c r="E22">
         <v>7.7126814006275586E-5</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>36428091.839511126</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <v>2809.5826639095012</v>
       </c>
       <c r="H22">
@@ -5042,10 +5073,10 @@
       <c r="E23">
         <v>1.791348259102799E-3</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>6906618.0694853142</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>12372.158255060451</v>
       </c>
       <c r="H23">
@@ -5068,10 +5099,10 @@
       <c r="E24">
         <v>8.0756148857289366E-5</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>31698095.08031968</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="3">
         <v>2559.816084798807</v>
       </c>
       <c r="H24">
@@ -5094,10 +5125,10 @@
       <c r="E25">
         <v>6.8692884514512029E-4</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>6413896.8770221323</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="3">
         <v>4405.890774612707</v>
       </c>
       <c r="H25">
@@ -5120,10 +5151,10 @@
       <c r="E26">
         <v>1.0944775283704231E-3</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>246476.5</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>269.76299052139251</v>
       </c>
     </row>
@@ -5143,10 +5174,10 @@
       <c r="E27">
         <v>1.090010807391068E-2</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>107667</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <v>1173.5819359937409</v>
       </c>
     </row>
@@ -5166,10 +5197,10 @@
       <c r="E28">
         <v>5.5523334435985628E-3</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3">
         <v>68683.310872100425</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="3">
         <v>381.35264397224</v>
       </c>
     </row>
@@ -5189,10 +5220,10 @@
       <c r="E29">
         <v>6.8692884514512029E-4</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3">
         <v>159857</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="3">
         <v>109.8103843983635</v>
       </c>
     </row>
@@ -5212,10 +5243,10 @@
       <c r="E30" s="2">
         <v>2.1118282427345699E-3</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="5">
         <v>21896431.973870799</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="5">
         <v>46241.503457536608</v>
       </c>
       <c r="H30" s="2">
@@ -5238,10 +5269,10 @@
       <c r="E31" s="2">
         <v>2.000886788871856E-2</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="5">
         <v>25577560.136865132</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="5">
         <v>511778.02169428871</v>
       </c>
       <c r="H31" s="2">
@@ -5264,10 +5295,10 @@
       <c r="E32" s="2">
         <v>5.5523334435985628E-3</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="5">
         <v>29024889.379979141</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="5">
         <v>161155.86400120691</v>
       </c>
       <c r="H32" s="2">
@@ -5290,10 +5321,10 @@
       <c r="E33" s="2">
         <v>2.5940985172919042E-3</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="5">
         <v>33392176.301814649</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="5">
         <v>86622.595033687234</v>
       </c>
       <c r="H33" s="2">
@@ -5316,10 +5347,10 @@
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="3">
         <v>2017068.655317503</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="3">
         <v>0</v>
       </c>
       <c r="H34">
@@ -5342,10 +5373,10 @@
       <c r="E35">
         <v>5.7883423581439412E-6</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="3">
         <v>2115740.8440453699</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="3">
         <v>12.246632346443031</v>
       </c>
       <c r="H35">
@@ -5368,10 +5399,10 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="3">
         <v>564901.33666130423</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="3">
         <v>0</v>
       </c>
     </row>
@@ -5391,10 +5422,10 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="3">
         <v>152326.6300376268</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="3">
         <v>0</v>
       </c>
     </row>
@@ -5414,10 +5445,10 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="3">
         <v>1264097.995133939</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="3">
         <v>0</v>
       </c>
       <c r="H38">
@@ -5440,10 +5471,10 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="3">
         <v>167204.17654073989</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="3">
         <v>0</v>
       </c>
     </row>
@@ -5463,10 +5494,10 @@
       <c r="E40">
         <v>5.9606897926980462E-4</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="3">
         <v>1519335.2860000001</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="3">
         <v>905.6286330946167</v>
       </c>
       <c r="H40">
@@ -5489,10 +5520,10 @@
       <c r="E41">
         <v>2.1123728539906361E-2</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="3">
         <v>19051</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="3">
         <v>402.42815241375598</v>
       </c>
     </row>
@@ -5512,10 +5543,10 @@
       <c r="E42">
         <v>2.1123728539906361E-2</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="3">
         <v>564641.01</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="3">
         <v>11927.323417738549</v>
       </c>
       <c r="H42">
@@ -5538,10 +5569,10 @@
       <c r="E43">
         <v>0</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="3">
         <v>31608</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="3">
         <v>0</v>
       </c>
       <c r="H43">
@@ -5564,10 +5595,10 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="3">
         <v>202455.1253333333</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="3">
         <v>0</v>
       </c>
       <c r="H44">
@@ -5590,10 +5621,10 @@
       <c r="E45">
         <v>0</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="3">
         <v>301461.19276470592</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="3">
         <v>0</v>
       </c>
       <c r="H45">
@@ -5616,10 +5647,10 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="3">
         <v>248842.38373118901</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="3">
         <v>0</v>
       </c>
       <c r="H46">
@@ -5642,10 +5673,10 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="3">
         <v>792319</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="3">
         <v>0</v>
       </c>
       <c r="H47">
@@ -5668,10 +5699,10 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="3">
         <v>1172545</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="3">
         <v>0</v>
       </c>
       <c r="H48">
@@ -5694,10 +5725,10 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="3">
         <v>1892795</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="3">
         <v>0</v>
       </c>
     </row>
@@ -5717,10 +5748,10 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="3">
         <v>20798650</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="3">
         <v>0</v>
       </c>
     </row>
@@ -5740,10 +5771,10 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="3">
         <v>12748261</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="3">
         <v>0</v>
       </c>
       <c r="H51">
@@ -5766,10 +5797,10 @@
       <c r="E52">
         <v>0</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="3">
         <v>11330218</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="3">
         <v>0</v>
       </c>
     </row>
@@ -5789,10 +5820,10 @@
       <c r="E53">
         <v>1.016309478451792E-4</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="3">
         <v>184727530.00525001</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="3">
         <v>18774.033967532341</v>
       </c>
       <c r="H53">
@@ -5815,10 +5846,10 @@
       <c r="E54">
         <v>3.0292449374460031E-5</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="3">
         <v>79784042.78475</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="3">
         <v>2416.8540769467918</v>
       </c>
       <c r="H54">
@@ -5841,10 +5872,10 @@
       <c r="E55">
         <v>6.4968500717780322E-6</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="3">
         <v>132614577.92729621</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="3">
         <v>861.57703012576758</v>
       </c>
       <c r="H55">
@@ -5867,10 +5898,10 @@
       <c r="E56">
         <v>4.0563463484641052E-5</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="3">
         <v>105493361.5907038</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="3">
         <v>4279.1761207565496</v>
       </c>
       <c r="H56">
@@ -5893,10 +5924,10 @@
       <c r="E57">
         <v>0</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="3">
         <v>156123</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="3">
         <v>0</v>
       </c>
     </row>
@@ -5916,10 +5947,10 @@
       <c r="E58">
         <v>0</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="3">
         <v>438704.72200000001</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="3">
         <v>0</v>
       </c>
       <c r="H58">
@@ -5942,10 +5973,10 @@
       <c r="E59">
         <v>6.6502380884435052E-6</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="3">
         <v>640539.32499999995</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="3">
         <v>4.2597390162608928</v>
       </c>
       <c r="H59">
@@ -5968,10 +5999,10 @@
       <c r="E60">
         <v>0</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="3">
         <v>79528</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="3">
         <v>0</v>
       </c>
     </row>
@@ -5991,10 +6022,10 @@
       <c r="E61">
         <v>0</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="3">
         <v>619909.95116279065</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="3">
         <v>0</v>
       </c>
     </row>
@@ -6014,10 +6045,10 @@
       <c r="E62">
         <v>0</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="3">
         <v>62199.4</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="3">
         <v>0</v>
       </c>
     </row>
@@ -6037,10 +6068,10 @@
       <c r="E63">
         <v>0</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="3">
         <v>492005.245</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="3">
         <v>0</v>
       </c>
     </row>
@@ -6060,10 +6091,10 @@
       <c r="E64">
         <v>0</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="3">
         <v>913348.23580446152</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="3">
         <v>0</v>
       </c>
       <c r="H64">
@@ -6086,10 +6117,10 @@
       <c r="E65">
         <v>0</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="3">
         <v>5900901.001218589</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="3">
         <v>0</v>
       </c>
       <c r="H65">
@@ -6112,10 +6143,10 @@
       <c r="E66">
         <v>1.5151059446953541E-5</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="3">
         <v>4739632.0318539664</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="3">
         <v>71.810446671304646</v>
       </c>
       <c r="H66">
@@ -6138,10 +6169,10 @@
       <c r="E67">
         <v>2.6667609846691722E-5</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="3">
         <v>4326410.9030381572</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="3">
         <v>115.37503799869479</v>
       </c>
       <c r="H67">
@@ -6164,10 +6195,10 @@
       <c r="E68">
         <v>1.0681139285240361E-6</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="3">
         <v>17226.322559848741</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="3">
         <v>1.8399675063422279E-2</v>
       </c>
     </row>
@@ -6187,10 +6218,10 @@
       <c r="E69">
         <v>0</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="3">
         <v>93717.001999999993</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="3">
         <v>0</v>
       </c>
     </row>
@@ -6210,10 +6241,10 @@
       <c r="E70">
         <v>2.4106733648042219E-5</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="3">
         <v>88026.33906281479</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="3">
         <v>2.1220275097995311</v>
       </c>
     </row>
@@ -6233,10 +6264,10 @@
       <c r="E71">
         <v>1.7175976198785941E-5</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="3">
         <v>27117.873653330069</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="3">
         <v>0.46577595243128161</v>
       </c>
     </row>
@@ -6256,10 +6287,10 @@
       <c r="E72">
         <v>2.1362278570480731E-6</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="3">
         <v>8190024.8600657582</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="3">
         <v>17.49575925598872</v>
       </c>
       <c r="H72">
@@ -6282,10 +6313,10 @@
       <c r="E73">
         <v>0</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="3">
         <v>4353366.5807391303</v>
       </c>
-      <c r="G73">
+      <c r="G73" s="3">
         <v>0</v>
       </c>
       <c r="H73">
@@ -6308,10 +6339,10 @@
       <c r="E74">
         <v>3.3062407849130902E-5</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="3">
         <v>10837196.79415895</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="3">
         <v>358.30382034977703</v>
       </c>
       <c r="H74">
@@ -6334,10 +6365,10 @@
       <c r="E75">
         <v>7.6843425508801645E-6</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="3">
         <v>2139314.2969999998</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="3">
         <v>16.439223882143381</v>
       </c>
       <c r="H75">
@@ -6353,9 +6384,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -6373,10 +6410,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -6399,10 +6436,10 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>2300</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>0</v>
       </c>
     </row>
@@ -6422,10 +6459,10 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>21469.262905162061</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -6445,10 +6482,10 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>753569.72512978013</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>0</v>
       </c>
       <c r="H4">
@@ -6471,10 +6508,10 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>700962.931795649</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>0</v>
       </c>
       <c r="H5">
@@ -6497,10 +6534,10 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>2452355.66145615</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>0</v>
       </c>
       <c r="H6">
@@ -6523,10 +6560,10 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>1761815.053452285</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>0</v>
       </c>
       <c r="H7">
@@ -6549,10 +6586,10 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>824600.54603952006</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>0</v>
       </c>
       <c r="H8">
@@ -6575,10 +6612,10 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>342935.35396048002</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>0</v>
       </c>
       <c r="H9">
@@ -6601,10 +6638,10 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>3597855.4026433248</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>0</v>
       </c>
       <c r="H10">
@@ -6627,10 +6664,10 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>371539.38865177229</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>0</v>
       </c>
       <c r="H11">
@@ -6653,10 +6690,10 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>2478138.821705427</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>0</v>
       </c>
     </row>
@@ -6676,10 +6713,10 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>18322212.479166672</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>0</v>
       </c>
       <c r="H13">
@@ -6702,10 +6739,10 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>6774519.576923077</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <v>0</v>
       </c>
       <c r="H14">
@@ -6728,10 +6765,10 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
         <v>0</v>
       </c>
     </row>
@@ -6751,10 +6788,10 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>38844786.131999999</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>0</v>
       </c>
       <c r="H16">
@@ -6777,10 +6814,10 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>15722</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>0</v>
       </c>
     </row>
@@ -6800,10 +6837,10 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>23373052.6192853</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>0</v>
       </c>
       <c r="H18">
@@ -6826,10 +6863,10 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>117464020.329</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>0</v>
       </c>
       <c r="H19">
@@ -6852,10 +6889,10 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>160428</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>0</v>
       </c>
     </row>
@@ -6875,10 +6912,10 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>22473219.009149559</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>0</v>
       </c>
       <c r="H21">
@@ -6901,10 +6938,10 @@
       <c r="E22">
         <v>6.9010075675589755E-5</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>36428091.839511126</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <v>2513.9053745619972</v>
       </c>
       <c r="H22">
@@ -6927,10 +6964,10 @@
       <c r="E23">
         <v>3.4115193104255872E-3</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>6906618.0694853142</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>23562.06091378344</v>
       </c>
       <c r="H23">
@@ -6953,10 +6990,10 @@
       <c r="E24">
         <v>2.0867652178946651E-4</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>31698095.08031968</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="3">
         <v>6614.6482287129093</v>
       </c>
       <c r="H24">
@@ -6979,10 +7016,10 @@
       <c r="E25">
         <v>2.4188189942729401E-3</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>6413896.8770221323</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="3">
         <v>15514.055593449029</v>
       </c>
       <c r="H25">
@@ -7005,10 +7042,10 @@
       <c r="E26">
         <v>7.95277733578326E-3</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>246476.5</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>1960.1727230031829</v>
       </c>
     </row>
@@ -7028,10 +7065,10 @@
       <c r="E27">
         <v>1.7456413613458271E-2</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>107667</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <v>1879.479684520212</v>
       </c>
     </row>
@@ -7051,10 +7088,10 @@
       <c r="E28">
         <v>3.9856207982979348E-2</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3">
         <v>68683.310872100425</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="3">
         <v>2737.4563230780609</v>
       </c>
     </row>
@@ -7074,10 +7111,10 @@
       <c r="E29">
         <v>2.4188189942729401E-3</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3">
         <v>159857</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="3">
         <v>386.66514796748942</v>
       </c>
     </row>
@@ -7097,10 +7134,10 @@
       <c r="E30">
         <v>1.5836544595890931E-2</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="3">
         <v>21896431.973870799</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="3">
         <v>346763.82144509692</v>
       </c>
       <c r="H30">
@@ -7123,10 +7160,10 @@
       <c r="E31">
         <v>3.1501307916490959E-2</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="3">
         <v>25577560.136865132</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="3">
         <v>805726.59762395313</v>
       </c>
       <c r="H31">
@@ -7149,10 +7186,10 @@
       <c r="E32">
         <v>3.9856207982979348E-2</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="3">
         <v>29024889.379979141</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="3">
         <v>1156822.0278114169</v>
       </c>
       <c r="H32">
@@ -7175,10 +7212,10 @@
       <c r="E33">
         <v>1.9483804256839439E-2</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="3">
         <v>33392176.301814649</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="3">
         <v>650606.62677442911</v>
       </c>
       <c r="H33">
@@ -7201,10 +7238,10 @@
       <c r="E34">
         <v>3.8871022846653247E-6</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="3">
         <v>2017068.655317503</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="3">
         <v>7.8405521784114809</v>
       </c>
       <c r="H34">
@@ -7227,10 +7264,10 @@
       <c r="E35">
         <v>5.7202442127540117E-5</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="3">
         <v>2115740.8440453699</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="3">
         <v>121.02554318837819</v>
       </c>
       <c r="H35">
@@ -7253,10 +7290,10 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="3">
         <v>564901.33666130423</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7276,10 +7313,10 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="3">
         <v>152326.6300376268</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7299,10 +7336,10 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="3">
         <v>1264097.995133939</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="3">
         <v>0</v>
       </c>
       <c r="H38">
@@ -7325,10 +7362,10 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="3">
         <v>167204.17654073989</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7348,10 +7385,10 @@
       <c r="E40">
         <v>6.9119918000175324E-3</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="3">
         <v>1519335.2860000001</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="3">
         <v>10501.63303830929</v>
       </c>
       <c r="H40">
@@ -7374,10 +7411,10 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="3">
         <v>19051</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7397,10 +7434,10 @@
       <c r="E42">
         <v>0</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="3">
         <v>564641.01</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="3">
         <v>0</v>
       </c>
       <c r="H42">
@@ -7423,10 +7460,10 @@
       <c r="E43">
         <v>0</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="3">
         <v>31608</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="3">
         <v>0</v>
       </c>
       <c r="H43">
@@ -7449,10 +7486,10 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="3">
         <v>202455.1253333333</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="3">
         <v>0</v>
       </c>
       <c r="H44">
@@ -7475,10 +7512,10 @@
       <c r="E45">
         <v>0</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="3">
         <v>301461.19276470592</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="3">
         <v>0</v>
       </c>
       <c r="H45">
@@ -7501,10 +7538,10 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="3">
         <v>248842.38373118901</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="3">
         <v>0</v>
       </c>
       <c r="H46">
@@ -7527,10 +7564,10 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="3">
         <v>792319</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="3">
         <v>0</v>
       </c>
       <c r="H47">
@@ -7553,10 +7590,10 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="3">
         <v>1172545</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="3">
         <v>0</v>
       </c>
       <c r="H48">
@@ -7579,10 +7616,10 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="3">
         <v>1892795</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7602,10 +7639,10 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="3">
         <v>20798650</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7625,10 +7662,10 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="3">
         <v>12748261</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="3">
         <v>0</v>
       </c>
       <c r="H51">
@@ -7651,10 +7688,10 @@
       <c r="E52">
         <v>0</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="3">
         <v>11330218</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7674,10 +7711,10 @@
       <c r="E53">
         <v>1.8776623969840581E-7</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="3">
         <v>184727530.00525001</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="3">
         <v>34.685593677860211</v>
       </c>
       <c r="H53">
@@ -7700,10 +7737,10 @@
       <c r="E54">
         <v>2.5890982371333359E-7</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="3">
         <v>79784042.78475</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="3">
         <v>20.656872452536689</v>
       </c>
       <c r="H54">
@@ -7726,10 +7763,10 @@
       <c r="E55">
         <v>1.0407575357702671E-6</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="3">
         <v>132614577.92729621</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="3">
         <v>138.01962133082679</v>
       </c>
       <c r="H55">
@@ -7752,10 +7789,10 @@
       <c r="E56">
         <v>1.9017094929508229E-8</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="3">
         <v>105493361.5907038</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="3">
         <v>2.0061772718033519</v>
       </c>
       <c r="H56">
@@ -7778,10 +7815,10 @@
       <c r="E57">
         <v>0</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="3">
         <v>156123</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7801,10 +7838,10 @@
       <c r="E58">
         <v>0</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="3">
         <v>438704.72200000001</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="3">
         <v>0</v>
       </c>
       <c r="H58">
@@ -7827,10 +7864,10 @@
       <c r="E59">
         <v>2.216746029481168E-6</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="3">
         <v>640539.32499999995</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="3">
         <v>1.419913005420298</v>
       </c>
       <c r="H59">
@@ -7853,10 +7890,10 @@
       <c r="E60">
         <v>0</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="3">
         <v>79528</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7876,10 +7913,10 @@
       <c r="E61">
         <v>0</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="3">
         <v>619909.95116279065</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7899,10 +7936,10 @@
       <c r="E62">
         <v>0</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="3">
         <v>62199.4</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7922,10 +7959,10 @@
       <c r="E63">
         <v>0</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="3">
         <v>492005.245</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="3">
         <v>0</v>
       </c>
     </row>
@@ -7945,10 +7982,10 @@
       <c r="E64">
         <v>0</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="3">
         <v>913348.23580446152</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="3">
         <v>0</v>
       </c>
       <c r="H64">
@@ -7971,10 +8008,10 @@
       <c r="E65">
         <v>3.1268862527593631E-6</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="3">
         <v>5900901.001218589</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="3">
         <v>18.451446219604371</v>
       </c>
       <c r="H65">
@@ -7997,10 +8034,10 @@
       <c r="E66">
         <v>6.3387085441336233E-6</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="3">
         <v>4739632.0318539664</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="3">
         <v>30.04314605636214</v>
       </c>
       <c r="H66">
@@ -8023,10 +8060,10 @@
       <c r="E67">
         <v>1.6000565908015041E-6</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="3">
         <v>4326410.9030381572</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="3">
         <v>6.9225022799216882</v>
       </c>
       <c r="H67">
@@ -8049,10 +8086,10 @@
       <c r="E68">
         <v>5.3405696426201816E-7</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="3">
         <v>17226.322559848741</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="3">
         <v>9.1998375317111376E-3</v>
       </c>
     </row>
@@ -8072,10 +8109,10 @@
       <c r="E69">
         <v>1.563443126379682E-6</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="3">
         <v>93717.001999999993</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="3">
         <v>0.1465212026018109</v>
       </c>
     </row>
@@ -8095,10 +8132,10 @@
       <c r="E70">
         <v>3.1693542720668121E-6</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="3">
         <v>88026.33906281479</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="3">
         <v>0.2789866537631337</v>
       </c>
     </row>
@@ -8118,10 +8155,10 @@
       <c r="E71">
         <v>8.0002829540075183E-7</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="3">
         <v>27117.873653330069</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="3">
         <v>2.1695066233766609E-2</v>
       </c>
     </row>
@@ -8141,10 +8178,10 @@
       <c r="E72">
         <v>1.0681139285240361E-6</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="3">
         <v>8190024.8600657582</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="3">
         <v>8.747879627994358</v>
       </c>
       <c r="H72">
@@ -8167,10 +8204,10 @@
       <c r="E73">
         <v>0</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="3">
         <v>4353366.5807391303</v>
       </c>
-      <c r="G73">
+      <c r="G73" s="3">
         <v>0</v>
       </c>
       <c r="H73">
@@ -8193,10 +8230,10 @@
       <c r="E74">
         <v>0</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="3">
         <v>10837196.79415895</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="3">
         <v>0</v>
       </c>
       <c r="H74">
@@ -8219,10 +8256,10 @@
       <c r="E75">
         <v>0</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="3">
         <v>2139314.2969999998</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="3">
         <v>0</v>
       </c>
       <c r="H75">
@@ -8306,9 +8343,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -8334,19 +8380,19 @@
       <c r="A2" t="s">
         <v>85</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>7426545</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>137813</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>3025979</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>10590337</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>4803.696062957024</v>
       </c>
     </row>
@@ -8354,19 +8400,19 @@
       <c r="A3" t="s">
         <v>86</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>11031839</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>95068</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>490416</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>11617323</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>5269.5290770444872</v>
       </c>
     </row>
@@ -8374,19 +8420,19 @@
       <c r="A4" t="s">
         <v>87</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>27279750</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>186489</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>870063</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>28336302</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>12853.130391994249</v>
       </c>
     </row>
@@ -8394,19 +8440,19 @@
       <c r="A5" t="s">
         <v>88</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>59884972</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>285</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>2715331</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>62600588</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>28395.149098125468</v>
       </c>
     </row>

</xml_diff>